<commit_message>
Added option to define weather data units.
</commit_message>
<xml_diff>
--- a/sites_in_prism_fao.xlsx
+++ b/sites_in_prism_fao.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Consumptive Use\CONS2_Python\cons2_v4 files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ProgrammingFolder\Repositories\cons2-python\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="9960" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15180" windowHeight="9960" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Agua Fria" sheetId="2" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="903" uniqueCount="88">
   <si>
     <t>HUC</t>
   </si>
@@ -324,6 +324,12 @@
   </si>
   <si>
     <t>Yavapi B</t>
+  </si>
+  <si>
+    <t>wx_units</t>
+  </si>
+  <si>
+    <t>metric</t>
   </si>
 </sst>
 </file>
@@ -651,10 +657,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet46"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,17 +751,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -767,10 +781,10 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet33"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,17 +875,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -883,10 +905,10 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet30"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,17 +999,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -999,10 +1029,10 @@
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet14"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,17 +1123,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1115,10 +1153,10 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet20"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1209,17 +1247,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1231,10 +1277,10 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet24"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1325,17 +1371,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1347,10 +1401,10 @@
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1441,17 +1495,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>28</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1463,10 +1525,10 @@
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet29"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,17 +1619,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1579,10 +1649,10 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1673,17 +1743,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1695,10 +1773,10 @@
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet26"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1789,17 +1867,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1811,10 +1897,10 @@
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet21"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1905,17 +1991,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1927,10 +2021,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet48"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2021,17 +2115,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2043,10 +2145,10 @@
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet41"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2137,17 +2239,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2159,10 +2269,10 @@
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet19"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2253,17 +2363,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2275,10 +2393,10 @@
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet18"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2369,17 +2487,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2391,10 +2517,10 @@
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet38"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2485,17 +2611,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2507,10 +2641,10 @@
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet27"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2601,17 +2735,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2623,10 +2765,10 @@
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet17"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2717,17 +2859,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2739,10 +2889,10 @@
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet15"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2833,17 +2983,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2855,10 +3013,10 @@
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet28"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2949,17 +3107,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -2971,10 +3137,10 @@
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet12"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3065,17 +3231,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -3087,10 +3261,10 @@
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet42"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3181,17 +3355,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -3203,10 +3385,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet47"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3297,17 +3479,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -3319,10 +3509,10 @@
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet11"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3413,17 +3603,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -3435,10 +3633,10 @@
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3529,17 +3727,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -3551,10 +3757,10 @@
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet44"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3645,17 +3851,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -3667,10 +3881,10 @@
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet45"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3761,17 +3975,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -3783,10 +4005,10 @@
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3877,17 +4099,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>30</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -3899,10 +4129,10 @@
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3993,17 +4223,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -4015,10 +4253,10 @@
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4108,17 +4346,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>86</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -4130,10 +4376,10 @@
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet39"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4224,17 +4470,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -4246,10 +4500,10 @@
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet37"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4340,17 +4594,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -4362,10 +4624,10 @@
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet49"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4456,17 +4718,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -4478,10 +4748,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet40"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4572,17 +4842,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -4593,10 +4871,10 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4687,17 +4965,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>21</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -4709,10 +4995,10 @@
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet43"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4803,17 +5089,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -4825,10 +5119,10 @@
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4919,17 +5213,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -4941,10 +5243,10 @@
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5035,17 +5337,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -5056,10 +5366,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5147,17 +5457,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -5169,10 +5487,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet32"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5263,17 +5581,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -5285,10 +5611,10 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet22"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5379,17 +5705,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -5401,10 +5735,10 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5495,17 +5829,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>86</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -5517,10 +5859,10 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet34"/>
-  <dimension ref="A2:I8"/>
+  <dimension ref="A2:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5611,17 +5953,25 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>82</v>
       </c>
     </row>

</xml_diff>